<commit_message>
added more series names
</commit_message>
<xml_diff>
--- a/HW_list.xlsx
+++ b/HW_list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ankur Ram\OneDrive\Desktop\Workspace\Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ankur Ram\OneDrive\Desktop\Workspace\Python\DieCastTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA4606E-79DA-4AD5-98F9-A1C2B3FACCAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20DCF5EE-A544-46CF-8512-8ECA435A6A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,9 +31,6 @@
     <t>Series</t>
   </si>
   <si>
-    <t>2020 Koenigsegg Jesko</t>
-  </si>
-  <si>
     <t>Mainlines</t>
   </si>
   <si>
@@ -245,6 +242,9 @@
   </si>
   <si>
     <t>Subaru WRX STI</t>
+  </si>
+  <si>
+    <t>20 Koenigsegg Jesko</t>
   </si>
 </sst>
 </file>
@@ -586,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -612,10 +612,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>74</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -623,10 +623,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -634,10 +634,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -645,10 +645,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -656,10 +656,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -667,10 +667,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -678,10 +678,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -689,10 +689,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -700,10 +700,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -711,10 +711,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -722,10 +722,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -733,10 +733,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -744,10 +744,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -755,10 +755,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -766,10 +766,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -777,10 +777,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -788,10 +788,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -799,10 +799,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -810,10 +810,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -821,10 +821,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -832,10 +832,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -843,10 +843,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -854,10 +854,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -865,10 +865,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -876,10 +876,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -887,10 +887,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -898,10 +898,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -909,10 +909,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" t="s">
         <v>31</v>
-      </c>
-      <c r="C29" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -920,10 +920,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" t="s">
         <v>33</v>
-      </c>
-      <c r="C30" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -931,10 +931,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -942,10 +942,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -953,10 +953,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -964,10 +964,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C34" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -975,10 +975,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -986,10 +986,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C36" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -997,10 +997,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C37" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -1008,10 +1008,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C38" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -1019,10 +1019,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C39" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -1030,10 +1030,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C40" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -1041,10 +1041,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C41" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -1052,10 +1052,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C42" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -1063,10 +1063,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" t="s">
         <v>47</v>
-      </c>
-      <c r="C43" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -1074,10 +1074,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -1085,10 +1085,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -1096,10 +1096,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C46" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -1107,10 +1107,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C47" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -1118,10 +1118,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C48" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -1129,10 +1129,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C49" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -1140,10 +1140,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C50" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -1151,10 +1151,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C51" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
@@ -1162,10 +1162,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C52" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
@@ -1173,10 +1173,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C53" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
@@ -1184,10 +1184,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C54" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
@@ -1195,10 +1195,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
+        <v>59</v>
+      </c>
+      <c r="C55" t="s">
         <v>60</v>
-      </c>
-      <c r="C55" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
@@ -1206,10 +1206,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C56" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
@@ -1217,10 +1217,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C57" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
@@ -1228,10 +1228,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C58" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
@@ -1239,10 +1239,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C59" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
@@ -1250,10 +1250,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C60" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
@@ -1261,10 +1261,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C61" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
@@ -1272,10 +1272,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C62" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
@@ -1283,10 +1283,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C63" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
@@ -1294,10 +1294,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C64" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
@@ -1305,10 +1305,10 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C65" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
@@ -1316,10 +1316,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C66" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
@@ -1327,10 +1327,10 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C67" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
@@ -1338,10 +1338,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C68" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
@@ -1349,10 +1349,10 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C69" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>